<commit_message>
1. added another variable managment that decided if the managment would be configured oob or not 2. updtaes gitigonre file
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\device_template_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\device_template_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E0010A-A680-4F49-850B-97A846EC7BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,10 +19,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
     <definedName name="groups">'Data types'!$E$6:$E$8</definedName>
+    <definedName name="managment">'Data types'!$H$6:$H$7</definedName>
     <definedName name="models">'Data types'!$F$6:$F$12</definedName>
     <definedName name="types">'Data types'!$G$6:$G$9</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,12 +36,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>root</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0" shapeId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -63,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -87,31 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>root:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-192.168.100.0/24</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -135,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -183,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -231,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -255,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -280,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I4" authorId="0" shapeId="0">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -309,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>junos</t>
   </si>
@@ -335,9 +313,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>cisco</t>
   </si>
   <si>
@@ -389,9 +364,6 @@
     <t>mgmt_dg</t>
   </si>
   <si>
-    <t>snmp_server_client</t>
-  </si>
-  <si>
     <t>mgmt_vlan</t>
   </si>
   <si>
@@ -413,9 +385,6 @@
     <t>england-london</t>
   </si>
   <si>
-    <t>192.168.100.0/24</t>
-  </si>
-  <si>
     <t>10.10.140.100</t>
   </si>
   <si>
@@ -489,12 +458,42 @@
   </si>
   <si>
     <t>vqfx-home</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>pt-sw-backup</t>
+  </si>
+  <si>
+    <t>pt</t>
+  </si>
+  <si>
+    <t>israel-pt</t>
+  </si>
+  <si>
+    <t>10.10.106.3</t>
+  </si>
+  <si>
+    <t>10.10.107.254</t>
+  </si>
+  <si>
+    <t>mgmt_srv</t>
+  </si>
+  <si>
+    <t>management</t>
+  </si>
+  <si>
+    <t>out of band</t>
+  </si>
+  <si>
+    <t>internal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -744,15 +743,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -846,6 +844,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -881,6 +896,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1056,51 +1088,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.77734375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.21875" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="15" customWidth="1"/>
     <col min="14" max="14" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.77734375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.21875" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.77734375" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.21875" style="15" customWidth="1"/>
-    <col min="23" max="23" width="11.88671875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.77734375" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="12.28515625" style="15" customWidth="1"/>
+    <col min="23" max="23" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
@@ -1109,86 +1141,86 @@
         <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="O1" s="5" t="s">
+      <c r="V1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="P1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="5" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F2" s="11"/>
+        <v>47</v>
+      </c>
+      <c r="F2" s="8"/>
       <c r="G2" s="11"/>
       <c r="H2" s="11"/>
-      <c r="I2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
@@ -1204,29 +1236,29 @@
       <c r="W2" s="11"/>
       <c r="X2" s="12"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="11"/>
+        <v>47</v>
+      </c>
+      <c r="F3" s="8"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
-      <c r="I3" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11" t="s">
+        <v>54</v>
+      </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
@@ -1242,113 +1274,151 @@
       <c r="W3" s="11"/>
       <c r="X3" s="12"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F4" s="11">
+        <v>47</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="11">
         <v>200</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="H4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="J4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="L4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>38</v>
       </c>
       <c r="O4" s="11">
         <v>106</v>
       </c>
       <c r="P4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="R4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="T4" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="U4" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="V4" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="W4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="S4" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="U4" s="11" t="s">
+      <c r="X4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="V4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="W4" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="X4" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="11">
+        <v>10</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="11">
+        <v>106</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T5" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U5" s="11"/>
       <c r="V5" s="11"/>
       <c r="W5" s="11"/>
       <c r="X5" s="12"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="11"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="11"/>
+      <c r="F6" s="8"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1368,13 +1438,13 @@
       <c r="W6" s="11"/>
       <c r="X6" s="12"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="11"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="11"/>
+      <c r="F7" s="8"/>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -1394,13 +1464,13 @@
       <c r="W7" s="11"/>
       <c r="X7" s="12"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="11"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="11"/>
+      <c r="F8" s="8"/>
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>
@@ -1420,13 +1490,13 @@
       <c r="W8" s="11"/>
       <c r="X8" s="12"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="11"/>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="8"/>
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
@@ -1446,13 +1516,13 @@
       <c r="W9" s="11"/>
       <c r="X9" s="12"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="11"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
-      <c r="F10" s="11"/>
+      <c r="F10" s="8"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -1472,13 +1542,13 @@
       <c r="W10" s="11"/>
       <c r="X10" s="12"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="11"/>
+      <c r="F11" s="8"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
       <c r="I11" s="11"/>
@@ -1498,13 +1568,13 @@
       <c r="W11" s="11"/>
       <c r="X11" s="12"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="11"/>
+      <c r="F12" s="8"/>
       <c r="G12" s="11"/>
       <c r="H12" s="11"/>
       <c r="I12" s="11"/>
@@ -1524,13 +1594,13 @@
       <c r="W12" s="11"/>
       <c r="X12" s="12"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="11"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="11"/>
+      <c r="F13" s="8"/>
       <c r="G13" s="11"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -1550,13 +1620,13 @@
       <c r="W13" s="11"/>
       <c r="X13" s="12"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="11"/>
+      <c r="F14" s="8"/>
       <c r="G14" s="11"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
@@ -1576,13 +1646,13 @@
       <c r="W14" s="11"/>
       <c r="X14" s="12"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="11"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="11"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
@@ -1602,13 +1672,13 @@
       <c r="W15" s="11"/>
       <c r="X15" s="12"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="11"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="11"/>
+      <c r="F16" s="8"/>
       <c r="G16" s="11"/>
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
@@ -1628,13 +1698,13 @@
       <c r="W16" s="11"/>
       <c r="X16" s="12"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="11"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="11"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="11"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11"/>
@@ -1654,13 +1724,13 @@
       <c r="W17" s="11"/>
       <c r="X17" s="12"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="11"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="11"/>
+      <c r="F18" s="8"/>
       <c r="G18" s="11"/>
       <c r="H18" s="11"/>
       <c r="I18" s="11"/>
@@ -1680,13 +1750,13 @@
       <c r="W18" s="11"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="11"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="11"/>
+      <c r="F19" s="8"/>
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="I19" s="11"/>
@@ -1706,13 +1776,13 @@
       <c r="W19" s="11"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="11"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="11"/>
+      <c r="F20" s="8"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -1732,13 +1802,13 @@
       <c r="W20" s="11"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="11"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="11"/>
+      <c r="F21" s="8"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -1758,13 +1828,13 @@
       <c r="W21" s="11"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="11"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="11"/>
+      <c r="F22" s="8"/>
       <c r="G22" s="11"/>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
@@ -1784,13 +1854,13 @@
       <c r="W22" s="11"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="11"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="11"/>
+      <c r="F23" s="8"/>
       <c r="G23" s="11"/>
       <c r="H23" s="11"/>
       <c r="I23" s="11"/>
@@ -1810,13 +1880,13 @@
       <c r="W23" s="11"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="11"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="11"/>
+      <c r="F24" s="8"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
@@ -1836,13 +1906,13 @@
       <c r="W24" s="11"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="11"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="11"/>
+      <c r="F25" s="8"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
       <c r="I25" s="11"/>
@@ -1862,13 +1932,13 @@
       <c r="W25" s="11"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="13"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
-      <c r="F26" s="13"/>
+      <c r="F26" s="10"/>
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
@@ -1889,17 +1959,20 @@
       <c r="X26" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E14"/>
+  <autoFilter ref="A1:E14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B5:B26">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 D5:D26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>models</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4 E5:E26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>types</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F26" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
+      <formula1>managment</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1910,122 +1983,142 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="E4:G17"/>
+  <dimension ref="E4:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E6" s="7" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E7" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E8" s="7" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="18"/>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E9" s="7"/>
       <c r="F9" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="18"/>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E10" s="7"/>
       <c r="F10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="17"/>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="8"/>
+      <c r="H10" s="18"/>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E11" s="7"/>
       <c r="F11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="17"/>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="8"/>
+      <c r="H11" s="18"/>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E12" s="7"/>
       <c r="F12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="17"/>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+      <c r="G12" s="8"/>
+      <c r="H12" s="18"/>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="17"/>
-    </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G13" s="8"/>
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="8"/>
+      <c r="H14" s="18"/>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="8"/>
+      <c r="H15" s="18"/>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
-      <c r="G16" s="17"/>
-    </row>
-    <row r="17" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G16" s="8"/>
+      <c r="H16" s="18"/>
+    </row>
+    <row r="17" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="18"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add the vault to the configuration and  changed junos config to override
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\device_template_config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\device_template_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E0010A-A680-4F49-850B-97A846EC7BD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41AF829-EBBE-413D-8875-8068954D0E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Data types" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
     <definedName name="groups">'Data types'!$E$6:$E$8</definedName>
     <definedName name="managment">'Data types'!$H$6:$H$7</definedName>
     <definedName name="models">'Data types'!$F$6:$F$12</definedName>
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
   <si>
     <t>junos</t>
   </si>
@@ -488,6 +488,39 @@
   </si>
   <si>
     <t>internal</t>
+  </si>
+  <si>
+    <t>pt-sw-accessR2</t>
+  </si>
+  <si>
+    <t>10.9.12.70</t>
+  </si>
+  <si>
+    <t>10.10.106.5</t>
+  </si>
+  <si>
+    <t>10.10.106.4</t>
+  </si>
+  <si>
+    <t>pt-sw-accessR1</t>
+  </si>
+  <si>
+    <t>pt-sw-accessR3</t>
+  </si>
+  <si>
+    <t>pt-sw-accessR4</t>
+  </si>
+  <si>
+    <t>pt-sw-accessR5</t>
+  </si>
+  <si>
+    <t>10.10.106.6</t>
+  </si>
+  <si>
+    <t>10.10.106.7</t>
+  </si>
+  <si>
+    <t>10.10.106.8</t>
   </si>
 </sst>
 </file>
@@ -498,26 +531,26 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1092,39 +1125,39 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X26"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.375" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.875" style="15" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.25" style="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" style="15" customWidth="1"/>
     <col min="14" max="14" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.28515625" style="15" customWidth="1"/>
-    <col min="23" max="23" width="11.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.25" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="12.25" style="15" customWidth="1"/>
+    <col min="23" max="23" width="11.875" style="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.75" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1198,7 +1231,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>52</v>
       </c>
@@ -1236,7 +1269,7 @@
       <c r="W2" s="11"/>
       <c r="X2" s="12"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>56</v>
       </c>
@@ -1274,7 +1307,7 @@
       <c r="W3" s="11"/>
       <c r="X3" s="12"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>29</v>
       </c>
@@ -1346,12 +1379,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>61</v>
@@ -1412,137 +1445,337 @@
       <c r="W5" s="11"/>
       <c r="X5" s="12"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="11">
+        <v>10</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="11">
+        <v>106</v>
+      </c>
+      <c r="P6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U6" s="11"/>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
       <c r="X6" s="12"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="11">
+        <v>10</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="11">
+        <v>106</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U7" s="11"/>
       <c r="V7" s="11"/>
       <c r="W7" s="11"/>
       <c r="X7" s="12"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="11">
+        <v>10</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="11">
+        <v>106</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q8" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U8" s="11"/>
       <c r="V8" s="11"/>
       <c r="W8" s="11"/>
       <c r="X8" s="12"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" s="11">
+        <v>10</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="11">
+        <v>106</v>
+      </c>
+      <c r="P9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q9" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R9" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U9" s="11"/>
       <c r="V9" s="11"/>
       <c r="W9" s="11"/>
       <c r="X9" s="12"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="11">
+        <v>10</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="11">
+        <v>106</v>
+      </c>
+      <c r="P10" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q10" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="R10" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T10" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="U10" s="11"/>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>
       <c r="X10" s="12"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="11"/>
@@ -1568,7 +1801,7 @@
       <c r="W11" s="11"/>
       <c r="X11" s="12"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="11"/>
@@ -1594,7 +1827,7 @@
       <c r="W12" s="11"/>
       <c r="X12" s="12"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="11"/>
@@ -1620,7 +1853,7 @@
       <c r="W13" s="11"/>
       <c r="X13" s="12"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="11"/>
@@ -1646,7 +1879,7 @@
       <c r="W14" s="11"/>
       <c r="X14" s="12"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="11"/>
@@ -1672,7 +1905,7 @@
       <c r="W15" s="11"/>
       <c r="X15" s="12"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="11"/>
@@ -1698,7 +1931,7 @@
       <c r="W16" s="11"/>
       <c r="X16" s="12"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="11"/>
@@ -1724,7 +1957,7 @@
       <c r="W17" s="11"/>
       <c r="X17" s="12"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="11"/>
@@ -1750,7 +1983,7 @@
       <c r="W18" s="11"/>
       <c r="X18" s="12"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="11"/>
@@ -1776,7 +2009,7 @@
       <c r="W19" s="11"/>
       <c r="X19" s="12"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="11"/>
@@ -1802,7 +2035,7 @@
       <c r="W20" s="11"/>
       <c r="X20" s="12"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="11"/>
@@ -1828,7 +2061,7 @@
       <c r="W21" s="11"/>
       <c r="X21" s="12"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="11"/>
@@ -1854,7 +2087,7 @@
       <c r="W22" s="11"/>
       <c r="X22" s="12"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="11"/>
@@ -1880,7 +2113,7 @@
       <c r="W23" s="11"/>
       <c r="X23" s="12"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="11"/>
@@ -1906,7 +2139,7 @@
       <c r="W24" s="11"/>
       <c r="X24" s="12"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="11"/>
@@ -1932,46 +2165,72 @@
       <c r="W25" s="11"/>
       <c r="X25" s="12"/>
     </row>
-    <row r="26" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="14"/>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11"/>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11"/>
+      <c r="X26" s="12"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="13"/>
+      <c r="X27" s="14"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E14" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>models</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F26" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
       <formula1>managment</formula1>
     </dataValidation>
   </dataValidations>
@@ -1993,16 +2252,16 @@
       <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="5:8" ht="15" x14ac:dyDescent="0.2">
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
@@ -2016,7 +2275,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E6" s="7" t="s">
         <v>0</v>
       </c>
@@ -2030,7 +2289,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E7" s="7" t="s">
         <v>8</v>
       </c>
@@ -2044,7 +2303,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E8" s="7" t="s">
         <v>57</v>
       </c>
@@ -2056,7 +2315,7 @@
       </c>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E9" s="7"/>
       <c r="F9" s="16" t="s">
         <v>44</v>
@@ -2066,7 +2325,7 @@
       </c>
       <c r="H9" s="18"/>
     </row>
-    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E10" s="7"/>
       <c r="F10" s="8" t="s">
         <v>4</v>
@@ -2074,7 +2333,7 @@
       <c r="G10" s="8"/>
       <c r="H10" s="18"/>
     </row>
-    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E11" s="7"/>
       <c r="F11" s="8" t="s">
         <v>6</v>
@@ -2082,7 +2341,7 @@
       <c r="G11" s="8"/>
       <c r="H11" s="18"/>
     </row>
-    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E12" s="7"/>
       <c r="F12" s="8" t="s">
         <v>11</v>
@@ -2090,31 +2349,31 @@
       <c r="G12" s="8"/>
       <c r="H12" s="18"/>
     </row>
-    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E13" s="7"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E14" s="7"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="18"/>
     </row>
-    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E15" s="7"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="18"/>
     </row>
-    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E16" s="7"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="18"/>
     </row>
-    <row r="17" spans="5:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>

</xml_diff>

<commit_message>
remove override from junos config and add some more variables to network devices excel file
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\device_template_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41AF829-EBBE-413D-8875-8068954D0E49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A3B69-A5D8-4F6D-99A0-742249F9AB4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Data types" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$G$15</definedName>
     <definedName name="groups">'Data types'!$E$6:$E$8</definedName>
     <definedName name="managment">'Data types'!$H$6:$H$7</definedName>
     <definedName name="models">'Data types'!$F$6:$F$12</definedName>
@@ -39,6 +39,8 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>root</author>
+    <author>tc={FBF01971-9F2D-4CAF-9739-59ADD8298FD6}</author>
+    <author>tc={A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -65,7 +67,23 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{FBF01971-9F2D-4CAF-9739-59ADD8298FD6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    install subnet ip</t>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    install default gateway</t>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -113,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +155,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -209,7 +227,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -258,7 +276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -287,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
   <si>
     <t>junos</t>
   </si>
@@ -521,13 +539,43 @@
   </si>
   <si>
     <t>10.10.106.8</t>
+  </si>
+  <si>
+    <t>10.9.12.43</t>
+  </si>
+  <si>
+    <t>10.9.12.47</t>
+  </si>
+  <si>
+    <t>10.9.13.201</t>
+  </si>
+  <si>
+    <t>10.9.13.202</t>
+  </si>
+  <si>
+    <t>ansible_host_dg</t>
+  </si>
+  <si>
+    <t>10.9.13.254</t>
+  </si>
+  <si>
+    <t>192.168.20.254</t>
+  </si>
+  <si>
+    <t>ansible_host_subnet</t>
+  </si>
+  <si>
+    <t>/24</t>
+  </si>
+  <si>
+    <t>/23</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +615,12 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="177"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -729,7 +783,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -738,15 +792,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -784,6 +829,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -799,6 +856,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Asher Bershtein" id="{C9B67452-23C3-4257-8C74-EB3FED103954}" userId="S::Asher.Bershtein@cellebrite.com::a540e936-a781-4e3e-993c-5a0495eb595d" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1120,1117 +1183,1230 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2020-06-25T23:18:44.99" personId="{C9B67452-23C3-4257-8C74-EB3FED103954}" id="{FBF01971-9F2D-4CAF-9739-59ADD8298FD6}">
+    <text>install subnet ip</text>
+  </threadedComment>
+  <threadedComment ref="E1" dT="2020-06-25T23:19:00.40" personId="{C9B67452-23C3-4257-8C74-EB3FED103954}" id="{A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}">
+    <text>install default gateway</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X27"/>
+  <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.125" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.375" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" style="15" customWidth="1"/>
-    <col min="7" max="7" width="10.125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19" style="15" customWidth="1"/>
-    <col min="14" max="14" width="10" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.25" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.75" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="12.25" style="15" customWidth="1"/>
-    <col min="23" max="23" width="11.875" style="15" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.75" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="12" customWidth="1"/>
+    <col min="4" max="4" width="12.125" style="12" customWidth="1"/>
+    <col min="5" max="5" width="16" style="12" customWidth="1"/>
+    <col min="6" max="6" width="10.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" style="12" customWidth="1"/>
+    <col min="16" max="16" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="12.25" style="12" customWidth="1"/>
+    <col min="25" max="25" width="11.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.75" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:26" s="20" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="I1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="J1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="N1" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="O1" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="P1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="Q1" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="V1" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="W1" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="X1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="Y1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Z1" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11" t="s">
+      <c r="H2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="12"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="9"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
       <c r="D3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="G3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11" t="s">
+      <c r="H3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="12"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="9"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="G4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="11">
+      <c r="H4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="8">
         <v>200</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="J4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="L4" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="M4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="N4" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="O4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="P4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="11">
+      <c r="Q4" s="8">
         <v>106</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="R4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="S4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="T4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S4" s="11" t="s">
+      <c r="U4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="T4" s="11" t="s">
+      <c r="V4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="W4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="V4" s="11" t="s">
+      <c r="X4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="11" t="s">
+      <c r="Y4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="Z4" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="8" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="H5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="11">
+      <c r="I5" s="8">
         <v>10</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="J5" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="K5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="L5" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="M5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="N5" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="O5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="11" t="s">
+      <c r="P5" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="11">
+      <c r="Q5" s="8">
         <v>106</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="R5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" s="11" t="s">
+      <c r="S5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="11" t="s">
+      <c r="T5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S5" s="11" t="s">
+      <c r="U5" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T5" s="11" t="s">
+      <c r="V5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="12"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="9"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="8">
+        <v>10</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>106</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="9"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="H7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="11">
+      <c r="I7" s="8">
         <v>10</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="J7" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="11" t="s">
+      <c r="K7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="L7" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="11" t="s">
+      <c r="M7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="11" t="s">
+      <c r="N7" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M6" s="11" t="s">
+      <c r="O7" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N6" s="11" t="s">
+      <c r="P7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O6" s="11">
+      <c r="Q7" s="8">
         <v>106</v>
       </c>
-      <c r="P6" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q6" s="11" t="s">
+      <c r="R7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="S7" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R6" s="11" t="s">
+      <c r="T7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="U7" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T6" s="11" t="s">
+      <c r="V7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="12"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="8" t="s">
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="9"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="H8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="11">
+      <c r="I8" s="8">
         <v>10</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="J8" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="11" t="s">
+      <c r="K8" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="L8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="11" t="s">
+      <c r="M8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="11" t="s">
+      <c r="N8" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M7" s="11" t="s">
+      <c r="O8" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N7" s="11" t="s">
+      <c r="P8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O7" s="11">
+      <c r="Q8" s="8">
         <v>106</v>
       </c>
-      <c r="P7" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q7" s="11" t="s">
+      <c r="R8" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="S8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="T8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S7" s="11" t="s">
+      <c r="U8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T7" s="11" t="s">
+      <c r="V8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="12"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="9"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="H9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G8" s="11">
+      <c r="I9" s="8">
         <v>10</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="J9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="K9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="L9" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="M9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L8" s="11" t="s">
+      <c r="N9" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="11" t="s">
+      <c r="O9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N8" s="11" t="s">
+      <c r="P9" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O8" s="11">
+      <c r="Q9" s="8">
         <v>106</v>
       </c>
-      <c r="P8" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q8" s="11" t="s">
+      <c r="R9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="S9" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="T9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S8" s="11" t="s">
+      <c r="U9" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T8" s="11" t="s">
+      <c r="V9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="12"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="G10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="H10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="G9" s="11">
+      <c r="I10" s="8">
         <v>10</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="J10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="K10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="L10" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="M10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L9" s="11" t="s">
+      <c r="N10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="M9" s="11" t="s">
+      <c r="O10" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="P10" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="O9" s="11">
+      <c r="Q10" s="8">
         <v>106</v>
       </c>
-      <c r="P9" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q9" s="11" t="s">
+      <c r="R10" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="S10" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="T10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="S9" s="11" t="s">
+      <c r="U10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="T9" s="11" t="s">
+      <c r="V10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="12"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="11">
-        <v>10</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="N10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="O10" s="11">
-        <v>106</v>
-      </c>
-      <c r="P10" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q10" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="S10" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="T10" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="12"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="11"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="9"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="12"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="11"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="9"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="12"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="11"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="9"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="12"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="11"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="9"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="12"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="11"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="12"/>
-    </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="11"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="12"/>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="11"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="9"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="12"/>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="11"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
+      <c r="U17" s="8"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="9"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="12"/>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="11"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="9"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="12"/>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="11"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+      <c r="Y19" s="8"/>
+      <c r="Z19" s="9"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="12"/>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="11"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="9"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="12"/>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="11"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="9"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="12"/>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="11"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="9"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="12"/>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="11"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="9"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="12"/>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="11"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="9"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="12"/>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="11"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+      <c r="T25" s="8"/>
+      <c r="U25" s="8"/>
+      <c r="V25" s="8"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="8"/>
+      <c r="Y25" s="8"/>
+      <c r="Z25" s="9"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="12"/>
-    </row>
-    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="13"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+      <c r="R26" s="8"/>
+      <c r="S26" s="8"/>
+      <c r="T26" s="8"/>
+      <c r="U26" s="8"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="8"/>
+      <c r="X26" s="8"/>
+      <c r="Y26" s="8"/>
+      <c r="Z26" s="9"/>
+    </row>
+    <row r="27" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="13"/>
-      <c r="X27" s="14"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10"/>
+      <c r="R27" s="10"/>
+      <c r="S27" s="10"/>
+      <c r="T27" s="10"/>
+      <c r="U27" s="10"/>
+      <c r="V27" s="10"/>
+      <c r="W27" s="10"/>
+      <c r="X27" s="10"/>
+      <c r="Y27" s="10"/>
+      <c r="Z27" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>models</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H27" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
       <formula1>managment</formula1>
     </dataValidation>
   </dataValidations>
@@ -2249,7 +2425,7 @@
   <dimension ref="E4:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2276,108 +2452,108 @@
       </c>
     </row>
     <row r="6" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="14" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="14" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="8" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="18"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E9" s="7"/>
-      <c r="F9" s="16" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="18"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E10" s="7"/>
-      <c r="F10" s="8" t="s">
+      <c r="E10" s="4"/>
+      <c r="F10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="18"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="15"/>
     </row>
     <row r="11" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E11" s="7"/>
-      <c r="F11" s="8" t="s">
+      <c r="E11" s="4"/>
+      <c r="F11" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="18"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="15"/>
     </row>
     <row r="12" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E12" s="7"/>
-      <c r="F12" s="8" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="18"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="15"/>
     </row>
     <row r="13" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E13" s="7"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="18"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="15"/>
     </row>
     <row r="14" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E14" s="7"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="18"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="15"/>
     </row>
     <row r="15" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="7"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="18"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="5:8" x14ac:dyDescent="0.2">
-      <c r="E16" s="7"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="18"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="15"/>
     </row>
     <row r="17" spans="5:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="E17" s="9"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="19"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changed that config is done over dhcp mgmt port
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\device_template_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516A3B69-A5D8-4F6D-99A0-742249F9AB4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3E5D5A-05C5-4F06-9F7B-2DACDEBAABC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Data types" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$G$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$E$15</definedName>
     <definedName name="groups">'Data types'!$E$6:$E$8</definedName>
     <definedName name="managment">'Data types'!$H$6:$H$7</definedName>
     <definedName name="models">'Data types'!$F$6:$F$12</definedName>
@@ -39,8 +39,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>root</author>
-    <author>tc={FBF01971-9F2D-4CAF-9739-59ADD8298FD6}</author>
-    <author>tc={A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}</author>
   </authors>
   <commentList>
     <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -67,23 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="1" shapeId="0" xr:uid="{FBF01971-9F2D-4CAF-9739-59ADD8298FD6}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    install subnet ip</t>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="2" shapeId="0" xr:uid="{A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    install default gateway</t>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +89,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +113,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -227,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -251,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -276,7 +258,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="J4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -305,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="82">
   <si>
     <t>junos</t>
   </si>
@@ -544,38 +526,20 @@
     <t>10.9.12.43</t>
   </si>
   <si>
-    <t>10.9.12.47</t>
-  </si>
-  <si>
-    <t>10.9.13.201</t>
-  </si>
-  <si>
-    <t>10.9.13.202</t>
-  </si>
-  <si>
-    <t>ansible_host_dg</t>
-  </si>
-  <si>
-    <t>10.9.13.254</t>
-  </si>
-  <si>
-    <t>192.168.20.254</t>
-  </si>
-  <si>
-    <t>ansible_host_subnet</t>
-  </si>
-  <si>
-    <t>/24</t>
-  </si>
-  <si>
-    <t>/23</t>
+    <t>10.9.12.26</t>
+  </si>
+  <si>
+    <t>10.9.12.17</t>
+  </si>
+  <si>
+    <t>10.9.12.80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,12 +578,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="177"/>
     </font>
   </fonts>
   <fills count="3">
@@ -859,9 +817,7 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Asher Bershtein" id="{C9B67452-23C3-4257-8C74-EB3FED103954}" userId="S::Asher.Bershtein@cellebrite.com::a540e936-a781-4e3e-993c-5a0495eb595d" providerId="AD"/>
-</personList>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1183,26 +1139,15 @@
 </a:theme>
 </file>
 
-<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D1" dT="2020-06-25T23:18:44.99" personId="{C9B67452-23C3-4257-8C74-EB3FED103954}" id="{FBF01971-9F2D-4CAF-9739-59ADD8298FD6}">
-    <text>install subnet ip</text>
-  </threadedComment>
-  <threadedComment ref="E1" dT="2020-06-25T23:19:00.40" personId="{C9B67452-23C3-4257-8C74-EB3FED103954}" id="{A8E639EE-270B-4BFE-ACFB-04197B7F9FA8}">
-    <text>install default gateway</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z27"/>
+  <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1210,30 +1155,28 @@
     <col min="1" max="1" width="15.125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.625" style="12" customWidth="1"/>
     <col min="3" max="3" width="14.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="12.125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="16" style="12" customWidth="1"/>
-    <col min="6" max="6" width="10.75" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.125" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.25" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.25" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19" style="12" customWidth="1"/>
-    <col min="16" max="16" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.625" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.75" style="12" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.75" style="12" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" style="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.75" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="24" width="12.25" style="12" customWidth="1"/>
-    <col min="25" max="25" width="11.875" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19" style="12" customWidth="1"/>
+    <col min="14" max="14" width="10" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.25" style="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.75" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="12.25" style="12" customWidth="1"/>
+    <col min="23" max="23" width="11.875" style="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.75" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="20" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" s="20" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>14</v>
       </c>
@@ -1244,76 +1187,70 @@
         <v>45</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M1" s="18" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="N1" s="18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O1" s="18" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="P1" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q1" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R1" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="S1" s="18" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="T1" s="18" t="s">
         <v>21</v>
       </c>
       <c r="U1" s="18" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="V1" s="18" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="W1" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="X1" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>52</v>
       </c>
@@ -1323,27 +1260,23 @@
       <c r="C2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>84</v>
+      <c r="D2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="J2" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="K2" s="8"/>
-      <c r="L2" s="8" t="s">
-        <v>51</v>
-      </c>
+      <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
       <c r="O2" s="8"/>
@@ -1355,11 +1288,9 @@
       <c r="U2" s="8"/>
       <c r="V2" s="8"/>
       <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="9"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X2" s="9"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>56</v>
       </c>
@@ -1369,27 +1300,23 @@
       <c r="C3" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>84</v>
+      <c r="D3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="5" t="s">
         <v>66</v>
       </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="K3" s="8"/>
-      <c r="L3" s="8" t="s">
-        <v>54</v>
-      </c>
+      <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
@@ -1401,11 +1328,9 @@
       <c r="U3" s="8"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
-      <c r="X3" s="8"/>
-      <c r="Y3" s="8"/>
-      <c r="Z3" s="9"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X3" s="9"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>29</v>
       </c>
@@ -1415,77 +1340,71 @@
       <c r="C4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>84</v>
+      <c r="D4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>47</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="8">
+      <c r="G4" s="8">
         <v>200</v>
       </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J4" s="8" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O4" s="8">
+        <v>106</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>106</v>
+        <v>36</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="T4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="W4" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="X4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y4" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="Z4" s="9" t="s">
+      <c r="X4" s="9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>58</v>
       </c>
@@ -1495,69 +1414,63 @@
       <c r="C5" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="G5" s="8">
+        <v>10</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="8">
+        <v>106</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="I5" s="8">
-        <v>10</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" s="8">
-        <v>106</v>
-      </c>
       <c r="R5" s="8" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="S5" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U5" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U5" s="8"/>
+      <c r="V5" s="8"/>
       <c r="W5" s="8"/>
-      <c r="X5" s="8"/>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="9"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X5" s="9"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>71</v>
       </c>
@@ -1567,69 +1480,63 @@
       <c r="C6" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>83</v>
+      <c r="D6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="8">
+      <c r="G6" s="8">
         <v>10</v>
       </c>
+      <c r="H6" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J6" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O6" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O6" s="8">
+        <v>106</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q6" s="8">
-        <v>106</v>
+        <v>70</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="R6" s="8" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="S6" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T6" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U6" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
       <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
-      <c r="Z6" s="9"/>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X6" s="9"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>67</v>
       </c>
@@ -1639,69 +1546,63 @@
       <c r="C7" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>83</v>
+      <c r="D7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I7" s="8">
+      <c r="G7" s="8">
         <v>10</v>
       </c>
+      <c r="H7" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J7" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N7" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O7" s="8">
+        <v>106</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q7" s="8">
-        <v>106</v>
+        <v>69</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="S7" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U7" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V7" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
       <c r="W7" s="8"/>
-      <c r="X7" s="8"/>
-      <c r="Y7" s="8"/>
-      <c r="Z7" s="9"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X7" s="9"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>72</v>
       </c>
@@ -1709,71 +1610,65 @@
         <v>0</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I8" s="8">
+      <c r="G8" s="8">
         <v>10</v>
       </c>
+      <c r="H8" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J8" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O8" s="8">
+        <v>106</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q8" s="8">
-        <v>106</v>
+        <v>75</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>75</v>
+        <v>38</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U8" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V8" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
       <c r="W8" s="8"/>
-      <c r="X8" s="8"/>
-      <c r="Y8" s="8"/>
-      <c r="Z8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X8" s="9"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>73</v>
       </c>
@@ -1783,69 +1678,63 @@
       <c r="C9" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>83</v>
+      <c r="D9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I9" s="8">
+      <c r="G9" s="8">
         <v>10</v>
       </c>
+      <c r="H9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J9" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N9" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O9" s="8">
+        <v>106</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q9" s="8">
-        <v>106</v>
+        <v>76</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T9" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
       <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
-      <c r="Y9" s="8"/>
-      <c r="Z9" s="9"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X9" s="9"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>74</v>
       </c>
@@ -1853,79 +1742,73 @@
         <v>0</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="I10" s="8">
+      <c r="G10" s="8">
         <v>10</v>
       </c>
+      <c r="H10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J10" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O10" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="O10" s="8">
+        <v>106</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q10" s="8">
-        <v>106</v>
+        <v>77</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="T10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="U10" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="V10" s="8" t="s">
-        <v>38</v>
-      </c>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
       <c r="W10" s="8"/>
-      <c r="X10" s="8"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="9"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X10" s="9"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
@@ -1941,19 +1824,17 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
       <c r="W11" s="8"/>
-      <c r="X11" s="8"/>
-      <c r="Y11" s="8"/>
-      <c r="Z11" s="9"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X11" s="9"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
@@ -1969,19 +1850,17 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
       <c r="W12" s="8"/>
-      <c r="X12" s="8"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="9"/>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X12" s="9"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
@@ -1997,19 +1876,17 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
       <c r="W13" s="8"/>
-      <c r="X13" s="8"/>
-      <c r="Y13" s="8"/>
-      <c r="Z13" s="9"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X13" s="9"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
@@ -2025,19 +1902,17 @@
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
       <c r="W14" s="8"/>
-      <c r="X14" s="8"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="9"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X14" s="9"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
       <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
@@ -2053,19 +1928,17 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
       <c r="W15" s="8"/>
-      <c r="X15" s="8"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="9"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X15" s="9"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
@@ -2081,19 +1954,17 @@
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
       <c r="W16" s="8"/>
-      <c r="X16" s="8"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="9"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X16" s="9"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
@@ -2109,19 +1980,17 @@
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
       <c r="W17" s="8"/>
-      <c r="X17" s="8"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="9"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X17" s="9"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
@@ -2137,19 +2006,17 @@
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
       <c r="W18" s="8"/>
-      <c r="X18" s="8"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="9"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X18" s="9"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
@@ -2165,19 +2032,17 @@
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
       <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="9"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X19" s="9"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
@@ -2193,19 +2058,17 @@
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
       <c r="W20" s="8"/>
-      <c r="X20" s="8"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="9"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X20" s="9"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
@@ -2221,19 +2084,17 @@
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
       <c r="W21" s="8"/>
-      <c r="X21" s="8"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="9"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X21" s="9"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
@@ -2249,19 +2110,17 @@
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
       <c r="W22" s="8"/>
-      <c r="X22" s="8"/>
-      <c r="Y22" s="8"/>
-      <c r="Z22" s="9"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X22" s="9"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5"/>
       <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
@@ -2277,19 +2136,17 @@
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
-      <c r="X23" s="8"/>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="9"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X23" s="9"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
@@ -2305,19 +2162,17 @@
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="8"/>
-      <c r="Y24" s="8"/>
-      <c r="Z24" s="9"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X24" s="9"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5"/>
       <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
@@ -2333,19 +2188,17 @@
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-      <c r="X25" s="8"/>
-      <c r="Y25" s="8"/>
-      <c r="Z25" s="9"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X25" s="9"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
@@ -2361,19 +2214,17 @@
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-      <c r="X26" s="8"/>
-      <c r="Y26" s="8"/>
-      <c r="Z26" s="9"/>
-    </row>
-    <row r="27" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="X26" s="9"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -2389,24 +2240,22 @@
       <c r="U27" s="10"/>
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="11"/>
+      <c r="X27" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E15" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B27" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>models</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G27" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E27" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H27" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F27" xr:uid="{7D89A031-F93F-41A2-89F6-C700A15C0C57}">
       <formula1>managment</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>